<commit_message>
updated employees && dtr
</commit_message>
<xml_diff>
--- a/build/classes/Files/DailyTimeRecord.xlsx
+++ b/build/classes/Files/DailyTimeRecord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kerjan\Desktop\Tapales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\MySys\IT2C-TAPALES-HRS\src\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FD1699E-A125-4DBE-A557-D7C84D0A3A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850830B6-4A0E-4DC7-B9BD-538C4D69251A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{11309B57-A2C4-4696-B1AE-D35C1AAA1361}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{11309B57-A2C4-4696-B1AE-D35C1AAA1361}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -122,9 +122,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -162,7 +162,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -268,7 +268,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -410,7 +410,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -421,7 +421,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,6 +738,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>